<commit_message>
Removed old postprocessing code
</commit_message>
<xml_diff>
--- a/channelsremoved.xlsx
+++ b/channelsremoved.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>7002</t>
   </si>
@@ -101,6 +101,39 @@
   </si>
   <si>
     <t>7065</t>
+  </si>
+  <si>
+    <t>7064</t>
+  </si>
+  <si>
+    <t>7065</t>
+  </si>
+  <si>
+    <t>7066</t>
+  </si>
+  <si>
+    <t>7067</t>
+  </si>
+  <si>
+    <t>7068</t>
+  </si>
+  <si>
+    <t>7069</t>
+  </si>
+  <si>
+    <t>7070</t>
+  </si>
+  <si>
+    <t>7071</t>
+  </si>
+  <si>
+    <t>7072</t>
+  </si>
+  <si>
+    <t>7073</t>
+  </si>
+  <si>
+    <t>7074</t>
   </si>
 </sst>
 </file>
@@ -493,7 +526,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B65"/>
+  <dimension ref="A2:B74"/>
   <sheetViews>
     <sheetView tabSelected="true" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="E57" sqref="E57"/>
@@ -707,17 +740,89 @@
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B64" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B65" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B72" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B74" s="0">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trying to figure out delay stuff
</commit_message>
<xml_diff>
--- a/channelsremoved.xlsx
+++ b/channelsremoved.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>7002</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>7082</t>
+  </si>
+  <si>
+    <t>7002</t>
+  </si>
+  <si>
+    <t>7023</t>
   </si>
 </sst>
 </file>
@@ -235,7 +241,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -259,11 +265,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -281,6 +291,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,11 +642,11 @@
   </cols>
   <sheetData>
     <row r="2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
+      <c r="A2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="23" x14ac:dyDescent="0.3">

</xml_diff>